<commit_message>
arrelgos página princiapl y graficos de asistencia
</commit_message>
<xml_diff>
--- a/public/uploads/Control KMS Ctto 4600020368 05-06-2023.xlsx
+++ b/public/uploads/Control KMS Ctto 4600020368 05-06-2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabri\Desktop\equipos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{098FF890-483A-4149-A989-AAA9B21DCACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72FF1E58-84D4-469B-A366-0E635EC21097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CAMI &amp; Equipos EECC" sheetId="1" r:id="rId1"/>
@@ -1671,11 +1671,11 @@
   </sheetPr>
   <dimension ref="A1:AY22"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J1" sqref="J1"/>
+      <selection pane="bottomRight" activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3482,8 +3482,8 @@
       <c r="AY22" s="17"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="K21">
-    <cfRule type="iconSet" priority="29">
+  <conditionalFormatting sqref="K18">
+    <cfRule type="iconSet" priority="13">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="TODAY()"/>
@@ -3491,17 +3491,8 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K21">
-    <cfRule type="iconSet" priority="28">
-      <iconSet iconSet="3Symbols">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="TODAY()"/>
-        <cfvo type="num" val="TODAY()+20"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K18">
-    <cfRule type="iconSet" priority="13">
+  <conditionalFormatting sqref="K19:K22">
+    <cfRule type="iconSet" priority="34">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="TODAY()"/>
@@ -3518,8 +3509,15 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K19:K22">
-    <cfRule type="iconSet" priority="34">
+  <conditionalFormatting sqref="K21">
+    <cfRule type="iconSet" priority="28">
+      <iconSet iconSet="3Symbols">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="TODAY()"/>
+        <cfvo type="num" val="TODAY()+20"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="29">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="TODAY()"/>
@@ -3962,8 +3960,8 @@
   </sheetPr>
   <dimension ref="A1:AQ116"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>